<commit_message>
docs: Add PortfolioDataMWRR requirements document.
</commit_message>
<xml_diff>
--- a/0. Requirements/PortfolioDataMWRR.xlsx
+++ b/0. Requirements/PortfolioDataMWRR.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB2FACB-0AA2-467A-9247-D684617784E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EE93A2-C7A2-4F23-ADAE-3BC0B3394A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$P$1:$AA$47</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -118,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="18">
   <si>
     <t>Descrizione Titolo</t>
   </si>
@@ -265,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,6 +294,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840B4B52-5CB9-41B5-89C1-B1D0A0795C06}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -834,38 +840,38 @@
         <v>8.0164948453608123E-2</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R3" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="7"/>
+      <c r="T3" s="7">
+        <v>242.5</v>
+      </c>
       <c r="U3" s="8">
-        <v>45383</v>
-      </c>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="9">
-        <v>30.01</v>
+        <v>45355</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="6">
+        <v>242.5</v>
+      </c>
+      <c r="X3" s="6">
+        <v>242.5</v>
       </c>
       <c r="Y3" s="10">
-        <f t="shared" ref="Y3:Y24" si="1">+X3*R3</f>
-        <v>23596.562900000001</v>
-      </c>
-      <c r="Z3" s="11">
-        <f>XIRR(_xlfn.VSTACK($J$29,Y3:Y3),_xlfn.VSTACK($F$29,U3:U3))</f>
-        <v>0.64926255345344552</v>
-      </c>
-      <c r="AA3" s="11">
-        <f>(Y3+$J$29)/ABS($J$2)</f>
-        <v>1.4344408689568931E-2</v>
-      </c>
+        <f>-X3*R3</f>
+        <v>-61941.047500000001</v>
+      </c>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -898,7 +904,7 @@
         <v>0.47180792689323425</v>
       </c>
       <c r="L4" s="11">
-        <f t="shared" ref="L4:L24" si="2">(J4+$J$2)/ABS($J$2)</f>
+        <f t="shared" ref="L4:L24" si="1">(J4+$J$2)/ABS($J$2)</f>
         <v>6.3340206185567072E-2</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -915,24 +921,24 @@
       </c>
       <c r="T4" s="7"/>
       <c r="U4" s="8">
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="9">
-        <v>29.79</v>
+        <v>30.01</v>
       </c>
       <c r="Y4" s="10">
-        <f t="shared" si="1"/>
-        <v>23423.579099999999</v>
+        <f>+X4*R4</f>
+        <v>23596.562900000001</v>
       </c>
       <c r="Z4" s="11">
-        <f t="shared" ref="Z4:Z24" si="3">XIRR(_xlfn.VSTACK($J$29,Y4:Y4),_xlfn.VSTACK($F$29,U4:U4))</f>
-        <v>0.21559515595436096</v>
+        <f>XIRR(_xlfn.VSTACK($Y$2:$Y$3,Y4:Y5),_xlfn.VSTACK($U$2:$U$3,U4:U5))</f>
+        <v>1.390959060192108</v>
       </c>
       <c r="AA4" s="11">
-        <f t="shared" ref="AA4:AA24" si="4">(Y4+$J$29)/ABS($J$2)</f>
-        <v>1.1551691953546639E-2</v>
+        <f>(Y4+$J$29)/ABS($J$2)</f>
+        <v>1.4344408689568931E-2</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
@@ -966,42 +972,36 @@
         <v>0.28520277142524719</v>
       </c>
       <c r="L5" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.3092783505154654E-2</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R5" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="8">
-        <v>45444</v>
-      </c>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
+        <v>45383</v>
+      </c>
+      <c r="V5" s="5"/>
+      <c r="W5" s="6"/>
       <c r="X5" s="9">
-        <v>28.84</v>
+        <v>261.94</v>
       </c>
       <c r="Y5" s="10">
-        <f t="shared" si="1"/>
-        <v>22676.603599999999</v>
-      </c>
-      <c r="Z5" s="11">
-        <f t="shared" si="3"/>
-        <v>-5.6680411100387572E-3</v>
-      </c>
-      <c r="AA5" s="11">
-        <f t="shared" si="4"/>
-        <v>-5.0776667927678054E-4</v>
-      </c>
+        <f>+X5*R5</f>
+        <v>66906.548379999993</v>
+      </c>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
@@ -1034,7 +1034,7 @@
         <v>-0.11233035288751125</v>
       </c>
       <c r="L6" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-3.8103092783505259E-2</v>
       </c>
       <c r="P6" s="4" t="s">
@@ -1051,24 +1051,24 @@
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="8">
-        <v>45474</v>
+        <v>45413</v>
       </c>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
       <c r="X6" s="9">
-        <v>29.31</v>
+        <v>29.79</v>
       </c>
       <c r="Y6" s="10">
-        <f t="shared" si="1"/>
-        <v>23046.159899999999</v>
+        <f>+X6*R6</f>
+        <v>23423.579099999999</v>
       </c>
       <c r="Z6" s="11">
-        <f t="shared" si="3"/>
-        <v>4.6375092864036557E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y6:Y6),_xlfn.VSTACK($F$29,U6:U6))</f>
+        <v>0.21559515595436096</v>
       </c>
       <c r="AA6" s="11">
-        <f t="shared" si="4"/>
-        <v>5.4584918022253315E-3</v>
+        <f>(Y6+$J$29)/ABS($J$2)</f>
+        <v>1.1551691953546639E-2</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
@@ -1098,46 +1098,40 @@
         <v>63734.145040000003</v>
       </c>
       <c r="K7" s="11">
-        <f t="shared" ref="K7:L24" si="5">XIRR(_xlfn.VSTACK($J$2:$J$2,J7:J7),_xlfn.VSTACK($F$2:$F$2,F7:F7))</f>
+        <f t="shared" ref="K7:L24" si="2">XIRR(_xlfn.VSTACK($J$2:$J$2,J7:J7),_xlfn.VSTACK($F$2:$F$2,F7:F7))</f>
         <v>7.1908727288246155E-2</v>
       </c>
       <c r="L7" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.8948453608247462E-2</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R7" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T7" s="7"/>
       <c r="U7" s="8">
-        <v>45505</v>
-      </c>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
+        <v>45413</v>
+      </c>
+      <c r="V7" s="5"/>
+      <c r="W7" s="6"/>
       <c r="X7" s="9">
-        <v>29.69</v>
+        <v>257.86</v>
       </c>
       <c r="Y7" s="10">
-        <f t="shared" si="1"/>
-        <v>23344.950099999998</v>
-      </c>
-      <c r="Z7" s="11">
-        <f t="shared" si="3"/>
-        <v>6.9625267386436471E-2</v>
-      </c>
-      <c r="AA7" s="11">
-        <f t="shared" si="4"/>
-        <v>1.0282275255354687E-2</v>
-      </c>
+        <f>+X7*R7</f>
+        <v>65864.406220000004</v>
+      </c>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
@@ -1166,11 +1160,11 @@
         <v>63463.392420000004</v>
       </c>
       <c r="K8" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>5.0181224942207336E-2</v>
       </c>
       <c r="L8" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.4577319587628918E-2</v>
       </c>
       <c r="P8" s="4" t="s">
@@ -1187,24 +1181,24 @@
       </c>
       <c r="T8" s="7"/>
       <c r="U8" s="8">
-        <v>45536</v>
+        <v>45444</v>
       </c>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="9">
-        <v>29.24</v>
+        <v>28.84</v>
       </c>
       <c r="Y8" s="10">
-        <f t="shared" si="1"/>
-        <v>22991.119599999998</v>
+        <f>+X8*R8</f>
+        <v>22676.603599999999</v>
       </c>
       <c r="Z8" s="11">
-        <f t="shared" si="3"/>
-        <v>2.5296637415885923E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y8:Y8),_xlfn.VSTACK($F$29,U8:U8))</f>
+        <v>-5.6680411100387572E-3</v>
       </c>
       <c r="AA8" s="11">
-        <f t="shared" si="4"/>
-        <v>4.5699001134909658E-3</v>
+        <f>(Y8+$J$29)/ABS($J$2)</f>
+        <v>-5.0776667927678054E-4</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
@@ -1234,46 +1228,40 @@
         <v>69529.78366999999</v>
       </c>
       <c r="K9" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.22130911946296689</v>
       </c>
       <c r="L9" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.1225154639175256</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R9" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="8">
-        <v>45566</v>
-      </c>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
+        <v>45444</v>
+      </c>
+      <c r="V9" s="5"/>
+      <c r="W9" s="6"/>
       <c r="X9" s="9">
-        <v>31.61</v>
+        <v>257.8</v>
       </c>
       <c r="Y9" s="10">
-        <f t="shared" si="1"/>
-        <v>24854.626899999999</v>
-      </c>
-      <c r="Z9" s="11">
-        <f t="shared" si="3"/>
-        <v>0.16911615729331972</v>
-      </c>
-      <c r="AA9" s="11">
-        <f t="shared" si="4"/>
-        <v>3.4655075860639914E-2</v>
-      </c>
+        <f>+X9*R9</f>
+        <v>65849.080600000001</v>
+      </c>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
@@ -1302,11 +1290,11 @@
         <v>61629.42656</v>
       </c>
       <c r="K10" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-7.5782626867294317E-3</v>
       </c>
       <c r="L10" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-5.0309278350515576E-3</v>
       </c>
       <c r="P10" s="4" t="s">
@@ -1323,24 +1311,24 @@
       </c>
       <c r="T10" s="7"/>
       <c r="U10" s="8">
-        <v>45597</v>
+        <v>45474</v>
       </c>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="9">
-        <v>30.82</v>
+        <v>29.31</v>
       </c>
       <c r="Y10" s="10">
-        <f t="shared" si="1"/>
-        <v>24233.4578</v>
+        <f>+X10*R10</f>
+        <v>23046.159899999999</v>
       </c>
       <c r="Z10" s="11">
-        <f t="shared" si="3"/>
-        <v>0.1030279576778412</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y10:Y10),_xlfn.VSTACK($F$29,U10:U10))</f>
+        <v>4.6375092864036557E-2</v>
       </c>
       <c r="AA10" s="11">
-        <f t="shared" si="4"/>
-        <v>2.4626683944923618E-2</v>
+        <f>(Y10+$J$29)/ABS($J$2)</f>
+        <v>5.4584918022253315E-3</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
@@ -1370,46 +1358,40 @@
         <v>61016.401760000001</v>
       </c>
       <c r="K11" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-1.9980546832084663E-2</v>
       </c>
       <c r="L11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.4927835051546391E-2</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R11" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T11" s="7"/>
       <c r="U11" s="8">
-        <v>45627</v>
-      </c>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
+        <v>45474</v>
+      </c>
+      <c r="V11" s="5"/>
+      <c r="W11" s="6"/>
       <c r="X11" s="9">
-        <v>32.200000000000003</v>
+        <v>233.26</v>
       </c>
       <c r="Y11" s="10">
-        <f t="shared" si="1"/>
-        <v>25318.538</v>
-      </c>
-      <c r="Z11" s="11">
-        <f t="shared" si="3"/>
-        <v>0.15722280144691467</v>
-      </c>
-      <c r="AA11" s="11">
-        <f t="shared" si="4"/>
-        <v>4.2144634379972366E-2</v>
-      </c>
+        <f>+X11*R11</f>
+        <v>59580.902019999994</v>
+      </c>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -1438,11 +1420,11 @@
         <v>60801.843079999999</v>
       </c>
       <c r="K12" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-2.2113189101219184E-2</v>
       </c>
       <c r="L12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.8391752577319617E-2</v>
       </c>
       <c r="P12" s="4" t="s">
@@ -1459,24 +1441,24 @@
       </c>
       <c r="T12" s="7"/>
       <c r="U12" s="8">
-        <v>45658</v>
+        <v>45505</v>
       </c>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="9">
-        <v>31.04</v>
+        <v>29.69</v>
       </c>
       <c r="Y12" s="10">
-        <f t="shared" si="1"/>
-        <v>24406.441599999998</v>
+        <f>+X12*R12</f>
+        <v>23344.950099999998</v>
       </c>
       <c r="Z12" s="11">
-        <f t="shared" si="3"/>
-        <v>9.0772452950477617E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y12:Y12),_xlfn.VSTACK($F$29,U12:U12))</f>
+        <v>6.9625267386436471E-2</v>
       </c>
       <c r="AA12" s="11">
-        <f t="shared" si="4"/>
-        <v>2.7419400680945852E-2</v>
+        <f>(Y12+$J$29)/ABS($J$2)</f>
+        <v>1.0282275255354687E-2</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
@@ -1506,46 +1488,40 @@
         <v>68132.597980000006</v>
       </c>
       <c r="K13" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.10972847342491152</v>
       </c>
       <c r="L13" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.9958762886598024E-2</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R13" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T13" s="7"/>
       <c r="U13" s="8">
-        <v>45689</v>
-      </c>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
+        <v>45505</v>
+      </c>
+      <c r="V13" s="5"/>
+      <c r="W13" s="6"/>
       <c r="X13" s="9">
-        <v>31.74</v>
+        <v>249.52</v>
       </c>
       <c r="Y13" s="10">
-        <f t="shared" si="1"/>
-        <v>24956.844599999997</v>
-      </c>
-      <c r="Z13" s="11">
-        <f t="shared" si="3"/>
-        <v>0.10870504975318909</v>
-      </c>
-      <c r="AA13" s="11">
-        <f t="shared" si="4"/>
-        <v>3.6305317568289391E-2</v>
-      </c>
+        <f>+X13*R13</f>
+        <v>63734.145040000003</v>
+      </c>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
@@ -1574,11 +1550,11 @@
         <v>73872.042669999995</v>
       </c>
       <c r="K14" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.19436083436012269</v>
       </c>
       <c r="L14" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.19261855670103084</v>
       </c>
       <c r="P14" s="4" t="s">
@@ -1595,24 +1571,24 @@
       </c>
       <c r="T14" s="7"/>
       <c r="U14" s="8">
-        <v>45717</v>
+        <v>45536</v>
       </c>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="9">
-        <v>31.45</v>
+        <v>29.24</v>
       </c>
       <c r="Y14" s="10">
-        <f t="shared" si="1"/>
-        <v>24728.820499999998</v>
+        <f>+X14*R14</f>
+        <v>22991.119599999998</v>
       </c>
       <c r="Z14" s="11">
-        <f t="shared" si="3"/>
-        <v>8.9758548140525821E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y14:Y14),_xlfn.VSTACK($F$29,U14:U14))</f>
+        <v>2.5296637415885923E-2</v>
       </c>
       <c r="AA14" s="11">
-        <f t="shared" si="4"/>
-        <v>3.2624009143532792E-2</v>
+        <f>(Y14+$J$29)/ABS($J$2)</f>
+        <v>4.5699001134909658E-3</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
@@ -1642,46 +1618,40 @@
         <v>76628.099999999991</v>
       </c>
       <c r="K15" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.2185002624988556</v>
       </c>
       <c r="L15" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.23711340206185552</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R15" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S15" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T15" s="7"/>
       <c r="U15" s="8">
-        <v>45748</v>
-      </c>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
+        <v>45536</v>
+      </c>
+      <c r="V15" s="5"/>
+      <c r="W15" s="6"/>
       <c r="X15" s="9">
-        <v>29.71</v>
+        <v>248.46</v>
       </c>
       <c r="Y15" s="10">
-        <f t="shared" si="1"/>
-        <v>23360.675899999998</v>
-      </c>
-      <c r="Z15" s="11">
-        <f t="shared" si="3"/>
-        <v>2.6664957404136665E-2</v>
-      </c>
-      <c r="AA15" s="11">
-        <f t="shared" si="4"/>
-        <v>1.0536158594993078E-2</v>
-      </c>
+        <f>+X15*R15</f>
+        <v>63463.392420000004</v>
+      </c>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -1710,11 +1680,11 @@
         <v>80280.706099999996</v>
       </c>
       <c r="K16" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.25080301165580754</v>
       </c>
       <c r="L16" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.29608247422680406</v>
       </c>
       <c r="P16" s="4" t="s">
@@ -1731,24 +1701,24 @@
       </c>
       <c r="T16" s="7"/>
       <c r="U16" s="8">
-        <v>45778</v>
+        <v>45566</v>
       </c>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="9">
-        <v>28.53</v>
+        <v>31.61</v>
       </c>
       <c r="Y16" s="10">
-        <f t="shared" si="1"/>
-        <v>22432.8537</v>
+        <f>+X16*R16</f>
+        <v>24854.626899999999</v>
       </c>
       <c r="Z16" s="11">
-        <f t="shared" si="3"/>
-        <v>-1.0466119647026064E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y16:Y16),_xlfn.VSTACK($F$29,U16:U16))</f>
+        <v>0.16911615729331972</v>
       </c>
       <c r="AA16" s="11">
-        <f t="shared" si="4"/>
-        <v>-4.4429584436717707E-3</v>
+        <f>(Y16+$J$29)/ABS($J$2)</f>
+        <v>3.4655075860639914E-2</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
@@ -1778,46 +1748,40 @@
         <v>81046.987099999998</v>
       </c>
       <c r="K17" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.24127950072288512</v>
       </c>
       <c r="L17" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.30845360824742263</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R17" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T17" s="7"/>
       <c r="U17" s="8">
-        <v>45809</v>
-      </c>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
+        <v>45566</v>
+      </c>
+      <c r="V17" s="5"/>
+      <c r="W17" s="6"/>
       <c r="X17" s="9">
-        <v>30.01</v>
+        <v>272.20999999999998</v>
       </c>
       <c r="Y17" s="10">
-        <f t="shared" si="1"/>
-        <v>23596.562900000001</v>
-      </c>
-      <c r="Z17" s="11">
-        <f t="shared" si="3"/>
-        <v>3.1338271498680112E-2</v>
-      </c>
-      <c r="AA17" s="11">
-        <f t="shared" si="4"/>
-        <v>1.4344408689568931E-2</v>
-      </c>
+        <f>+X17*R17</f>
+        <v>69529.78366999999</v>
+      </c>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
@@ -1846,11 +1810,11 @@
         <v>82296.025129999995</v>
       </c>
       <c r="K18" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.23896818757057189</v>
       </c>
       <c r="L18" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32861855670103085</v>
       </c>
       <c r="P18" s="4" t="s">
@@ -1867,24 +1831,24 @@
       </c>
       <c r="T18" s="7"/>
       <c r="U18" s="8">
-        <v>45839</v>
+        <v>45597</v>
       </c>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="9">
-        <v>29.99</v>
+        <v>30.82</v>
       </c>
       <c r="Y18" s="10">
-        <f t="shared" si="1"/>
-        <v>23580.837099999997</v>
+        <f>+X18*R18</f>
+        <v>24233.4578</v>
       </c>
       <c r="Z18" s="11">
-        <f t="shared" si="3"/>
-        <v>2.8850188851356512E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y18:Y18),_xlfn.VSTACK($F$29,U18:U18))</f>
+        <v>0.1030279576778412</v>
       </c>
       <c r="AA18" s="11">
-        <f t="shared" si="4"/>
-        <v>1.4090525349930482E-2</v>
+        <f>(Y18+$J$29)/ABS($J$2)</f>
+        <v>2.4626683944923618E-2</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
@@ -1914,46 +1878,40 @@
         <v>81046.987099999998</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.20990437865257267</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.30845360824742263</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R19" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S19" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T19" s="7"/>
       <c r="U19" s="8">
-        <v>45870</v>
-      </c>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
+        <v>45597</v>
+      </c>
+      <c r="V19" s="5"/>
+      <c r="W19" s="6"/>
       <c r="X19" s="9">
-        <v>31.68</v>
+        <v>241.28</v>
       </c>
       <c r="Y19" s="10">
-        <f t="shared" si="1"/>
-        <v>24909.6672</v>
-      </c>
-      <c r="Z19" s="11">
-        <f t="shared" si="3"/>
-        <v>6.7782369256019603E-2</v>
-      </c>
-      <c r="AA19" s="11">
-        <f t="shared" si="4"/>
-        <v>3.5543667549374283E-2</v>
-      </c>
+        <f>+X19*R19</f>
+        <v>61629.42656</v>
+      </c>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
@@ -1982,11 +1940,11 @@
         <v>86791.540330000003</v>
       </c>
       <c r="K20" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.25295136570930477</v>
       </c>
       <c r="L20" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.40119587628865983</v>
       </c>
       <c r="P20" s="4" t="s">
@@ -2003,24 +1961,24 @@
       </c>
       <c r="T20" s="7"/>
       <c r="U20" s="8">
-        <v>45901</v>
+        <v>45627</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="9">
-        <v>32.18</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="Y20" s="10">
-        <f t="shared" si="1"/>
-        <v>25302.8122</v>
+        <f>+X20*R20</f>
+        <v>25318.538</v>
       </c>
       <c r="Z20" s="11">
-        <f t="shared" si="3"/>
-        <v>7.500865757465365E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y20:Y20),_xlfn.VSTACK($F$29,U20:U20))</f>
+        <v>0.15722280144691467</v>
       </c>
       <c r="AA20" s="11">
-        <f t="shared" si="4"/>
-        <v>4.1890751040333976E-2</v>
+        <f>(Y20+$J$29)/ABS($J$2)</f>
+        <v>4.2144634379972366E-2</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.35">
@@ -2050,46 +2008,40 @@
         <v>87728.957419999992</v>
       </c>
       <c r="K21" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.24678036570549011</v>
       </c>
       <c r="L21" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.41632989690721633</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R21" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S21" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T21" s="7"/>
       <c r="U21" s="8">
-        <v>45931</v>
-      </c>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
+        <v>45627</v>
+      </c>
+      <c r="V21" s="5"/>
+      <c r="W21" s="6"/>
       <c r="X21" s="9">
-        <v>33.630000000000003</v>
+        <v>238.88</v>
       </c>
       <c r="Y21" s="10">
-        <f t="shared" si="1"/>
-        <v>26442.932700000001</v>
-      </c>
-      <c r="Z21" s="11">
-        <f t="shared" si="3"/>
-        <v>0.1012986123561859</v>
-      </c>
-      <c r="AA21" s="11">
-        <f t="shared" si="4"/>
-        <v>6.0297293164117097E-2</v>
-      </c>
+        <f>+X21*R21</f>
+        <v>61016.401760000001</v>
+      </c>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -2118,11 +2070,11 @@
         <v>85647.227369999993</v>
       </c>
       <c r="K22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.21514006257057192</v>
       </c>
       <c r="L22" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.38272164948453596</v>
       </c>
       <c r="P22" s="4" t="s">
@@ -2139,24 +2091,24 @@
       </c>
       <c r="T22" s="7"/>
       <c r="U22" s="8">
-        <v>45962</v>
+        <v>45658</v>
       </c>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
       <c r="X22" s="9">
-        <v>33.44</v>
+        <v>31.04</v>
       </c>
       <c r="Y22" s="10">
-        <f t="shared" si="1"/>
-        <v>26293.537599999996</v>
+        <f>+X22*R22</f>
+        <v>24406.441599999998</v>
       </c>
       <c r="Z22" s="11">
-        <f t="shared" si="3"/>
-        <v>9.2157724499702456E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y22:Y22),_xlfn.VSTACK($F$29,U22:U22))</f>
+        <v>9.0772452950477617E-2</v>
       </c>
       <c r="AA22" s="11">
-        <f t="shared" si="4"/>
-        <v>5.7885401437552331E-2</v>
+        <f>(Y22+$J$29)/ABS($J$2)</f>
+        <v>2.7419400680945852E-2</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
@@ -2186,46 +2138,40 @@
         <v>89550.151929999993</v>
       </c>
       <c r="K23" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.23517941832542419</v>
       </c>
       <c r="L23" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.44573195876288646</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R23" s="7">
-        <v>786.29</v>
+        <v>255.42699999999999</v>
       </c>
       <c r="S23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="T23" s="7"/>
       <c r="U23" s="8">
-        <v>45992</v>
-      </c>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
+        <v>45658</v>
+      </c>
+      <c r="V23" s="5"/>
+      <c r="W23" s="6"/>
       <c r="X23" s="9">
-        <v>33.11</v>
+        <v>238.04</v>
       </c>
       <c r="Y23" s="10">
-        <f t="shared" si="1"/>
-        <v>26034.061899999997</v>
-      </c>
-      <c r="Z23" s="11">
-        <f t="shared" si="3"/>
-        <v>8.1469628214836123E-2</v>
-      </c>
-      <c r="AA23" s="11">
-        <f t="shared" si="4"/>
-        <v>5.3696326333518951E-2</v>
-      </c>
+        <f>+X23*R23</f>
+        <v>60801.843079999999</v>
+      </c>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
@@ -2254,11 +2200,11 @@
         <v>92459.465460000007</v>
       </c>
       <c r="K24" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.24468657374382013</v>
       </c>
       <c r="L24" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.49270103092783513</v>
       </c>
       <c r="P24" s="4" t="s">
@@ -2275,24 +2221,115 @@
       </c>
       <c r="T24" s="7"/>
       <c r="U24" s="8">
-        <v>46023</v>
+        <v>45689</v>
       </c>
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="9">
-        <v>32.229999999999997</v>
+        <v>31.74</v>
       </c>
       <c r="Y24" s="10">
-        <f t="shared" si="1"/>
-        <v>25342.126699999997</v>
+        <f>+X24*R24</f>
+        <v>24956.844599999997</v>
       </c>
       <c r="Z24" s="11">
-        <f t="shared" si="3"/>
-        <v>6.18018299341202E-2</v>
+        <f>XIRR(_xlfn.VSTACK($J$29,Y24:Y24),_xlfn.VSTACK($F$29,U24:U24))</f>
+        <v>0.10870504975318909</v>
       </c>
       <c r="AA24" s="11">
-        <f t="shared" si="4"/>
-        <v>4.2525459389429893E-2</v>
+        <f>(Y24+$J$29)/ABS($J$2)</f>
+        <v>3.6305317568289391E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R25" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T25" s="7"/>
+      <c r="U25" s="8">
+        <v>45689</v>
+      </c>
+      <c r="V25" s="5"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="9">
+        <v>266.74</v>
+      </c>
+      <c r="Y25" s="10">
+        <f>+X25*R25</f>
+        <v>68132.597980000006</v>
+      </c>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T26" s="7"/>
+      <c r="U26" s="8">
+        <v>45717</v>
+      </c>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="9">
+        <v>31.45</v>
+      </c>
+      <c r="Y26" s="10">
+        <f>+X26*R26</f>
+        <v>24728.820499999998</v>
+      </c>
+      <c r="Z26" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y26:Y26),_xlfn.VSTACK($F$29,U26:U26))</f>
+        <v>8.9758548140525821E-2</v>
+      </c>
+      <c r="AA26" s="13">
+        <f>(Y26+$J$29)/ABS($J$2)</f>
+        <v>3.2624009143532792E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R27" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T27" s="7"/>
+      <c r="U27" s="8">
+        <v>45717</v>
+      </c>
+      <c r="V27" s="5"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="9">
+        <v>289.20999999999998</v>
+      </c>
+      <c r="Y27" s="10">
+        <f>+X27*R27</f>
+        <v>73872.042669999995</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.35">
@@ -2332,6 +2369,39 @@
       <c r="L28" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="P28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R28" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T28" s="7"/>
+      <c r="U28" s="8">
+        <v>45748</v>
+      </c>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="9">
+        <v>29.71</v>
+      </c>
+      <c r="Y28" s="10">
+        <f>+X28*R28</f>
+        <v>23360.675899999998</v>
+      </c>
+      <c r="Z28" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y28:Y28),_xlfn.VSTACK($F$29,U28:U28))</f>
+        <v>2.6664957404136665E-2</v>
+      </c>
+      <c r="AA28" s="13">
+        <f>(Y28+$J$29)/ABS($J$2)</f>
+        <v>1.0536158594993078E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
@@ -2367,6 +2437,31 @@
       </c>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
+      <c r="P29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R29" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T29" s="7"/>
+      <c r="U29" s="8">
+        <v>45748</v>
+      </c>
+      <c r="V29" s="5"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="9">
+        <v>300</v>
+      </c>
+      <c r="Y29" s="10">
+        <f>+X29*R29</f>
+        <v>76628.099999999991</v>
+      </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
@@ -2391,7 +2486,7 @@
         <v>30.01</v>
       </c>
       <c r="J30" s="10">
-        <f t="shared" ref="J30:J51" si="6">+I30*C30</f>
+        <f t="shared" ref="J30:J51" si="3">+I30*C30</f>
         <v>23596.562900000001</v>
       </c>
       <c r="K30" s="11">
@@ -2401,6 +2496,39 @@
       <c r="L30" s="11">
         <f>(J30+$J$29)/ABS($J$2)</f>
         <v>1.4344408689568931E-2</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R30" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T30" s="7"/>
+      <c r="U30" s="8">
+        <v>45778</v>
+      </c>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="9">
+        <v>28.53</v>
+      </c>
+      <c r="Y30" s="10">
+        <f>+X30*R30</f>
+        <v>22432.8537</v>
+      </c>
+      <c r="Z30" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y30:Y30),_xlfn.VSTACK($F$29,U30:U30))</f>
+        <v>-1.0466119647026064E-2</v>
+      </c>
+      <c r="AA30" s="13">
+        <f>(Y30+$J$29)/ABS($J$2)</f>
+        <v>-4.4429584436717707E-3</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.35">
@@ -2426,16 +2554,41 @@
         <v>29.79</v>
       </c>
       <c r="J31" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>23423.579099999999</v>
       </c>
       <c r="K31" s="11">
-        <f t="shared" ref="K31:K51" si="7">XIRR(_xlfn.VSTACK($J$29,J31:J31),_xlfn.VSTACK($F$29,F31:F31))</f>
+        <f t="shared" ref="K31:K51" si="4">XIRR(_xlfn.VSTACK($J$29,J31:J31),_xlfn.VSTACK($F$29,F31:F31))</f>
         <v>0.21559515595436096</v>
       </c>
       <c r="L31" s="11">
-        <f t="shared" ref="L31:L51" si="8">(J31+$J$29)/ABS($J$2)</f>
+        <f t="shared" ref="L31:L51" si="5">(J31+$J$29)/ABS($J$2)</f>
         <v>1.1551691953546639E-2</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R31" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T31" s="7"/>
+      <c r="U31" s="8">
+        <v>45778</v>
+      </c>
+      <c r="V31" s="5"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="9">
+        <v>314.3</v>
+      </c>
+      <c r="Y31" s="10">
+        <f>+X31*R31</f>
+        <v>80280.706099999996</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
@@ -2461,19 +2614,52 @@
         <v>28.84</v>
       </c>
       <c r="J32" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>22676.603599999999</v>
       </c>
       <c r="K32" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>-5.6680411100387572E-3</v>
       </c>
       <c r="L32" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>-5.0776667927678054E-4</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R32" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T32" s="7"/>
+      <c r="U32" s="8">
+        <v>45809</v>
+      </c>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="9">
+        <v>30.01</v>
+      </c>
+      <c r="Y32" s="10">
+        <f>+X32*R32</f>
+        <v>23596.562900000001</v>
+      </c>
+      <c r="Z32" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y32:Y32),_xlfn.VSTACK($F$29,U32:U32))</f>
+        <v>3.1338271498680112E-2</v>
+      </c>
+      <c r="AA32" s="13">
+        <f>(Y32+$J$29)/ABS($J$2)</f>
+        <v>1.4344408689568931E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>17</v>
       </c>
@@ -2496,19 +2682,44 @@
         <v>29.31</v>
       </c>
       <c r="J33" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>23046.159899999999</v>
       </c>
       <c r="K33" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4.6375092864036557E-2</v>
       </c>
       <c r="L33" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>5.4584918022253315E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R33" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T33" s="7"/>
+      <c r="U33" s="8">
+        <v>45809</v>
+      </c>
+      <c r="V33" s="5"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="9">
+        <v>317.3</v>
+      </c>
+      <c r="Y33" s="10">
+        <f>+X33*R33</f>
+        <v>81046.987099999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>17</v>
       </c>
@@ -2531,19 +2742,52 @@
         <v>29.69</v>
       </c>
       <c r="J34" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>23344.950099999998</v>
       </c>
       <c r="K34" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>6.9625267386436471E-2</v>
       </c>
       <c r="L34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.0282275255354687E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R34" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T34" s="7"/>
+      <c r="U34" s="8">
+        <v>45839</v>
+      </c>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="9">
+        <v>29.99</v>
+      </c>
+      <c r="Y34" s="10">
+        <f>+X34*R34</f>
+        <v>23580.837099999997</v>
+      </c>
+      <c r="Z34" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y34:Y34),_xlfn.VSTACK($F$29,U34:U34))</f>
+        <v>2.8850188851356512E-2</v>
+      </c>
+      <c r="AA34" s="13">
+        <f>(Y34+$J$29)/ABS($J$2)</f>
+        <v>1.4090525349930482E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>17</v>
       </c>
@@ -2566,19 +2810,44 @@
         <v>29.24</v>
       </c>
       <c r="J35" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>22991.119599999998</v>
       </c>
       <c r="K35" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2.5296637415885923E-2</v>
       </c>
       <c r="L35" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>4.5699001134909658E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R35" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T35" s="7"/>
+      <c r="U35" s="8">
+        <v>45839</v>
+      </c>
+      <c r="V35" s="5"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="9">
+        <v>322.19</v>
+      </c>
+      <c r="Y35" s="10">
+        <f>+X35*R35</f>
+        <v>82296.025129999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>17</v>
       </c>
@@ -2601,19 +2870,52 @@
         <v>31.61</v>
       </c>
       <c r="J36" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>24854.626899999999</v>
       </c>
       <c r="K36" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.16911615729331972</v>
       </c>
       <c r="L36" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3.4655075860639914E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R36" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T36" s="7"/>
+      <c r="U36" s="8">
+        <v>45870</v>
+      </c>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="9">
+        <v>31.68</v>
+      </c>
+      <c r="Y36" s="10">
+        <f>+X36*R36</f>
+        <v>24909.6672</v>
+      </c>
+      <c r="Z36" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y36:Y36),_xlfn.VSTACK($F$29,U36:U36))</f>
+        <v>6.7782369256019603E-2</v>
+      </c>
+      <c r="AA36" s="13">
+        <f>(Y36+$J$29)/ABS($J$2)</f>
+        <v>3.5543667549374283E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>17</v>
       </c>
@@ -2636,19 +2938,44 @@
         <v>30.82</v>
       </c>
       <c r="J37" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>24233.4578</v>
       </c>
       <c r="K37" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.1030279576778412</v>
       </c>
       <c r="L37" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2.4626683944923618E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R37" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T37" s="7"/>
+      <c r="U37" s="8">
+        <v>45870</v>
+      </c>
+      <c r="V37" s="5"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="9">
+        <v>317.3</v>
+      </c>
+      <c r="Y37" s="10">
+        <f>+X37*R37</f>
+        <v>81046.987099999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>17</v>
       </c>
@@ -2671,19 +2998,52 @@
         <v>32.200000000000003</v>
       </c>
       <c r="J38" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>25318.538</v>
       </c>
       <c r="K38" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.15722280144691467</v>
       </c>
       <c r="L38" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>4.2144634379972366E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R38" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T38" s="7"/>
+      <c r="U38" s="8">
+        <v>45901</v>
+      </c>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="9">
+        <v>32.18</v>
+      </c>
+      <c r="Y38" s="10">
+        <f>+X38*R38</f>
+        <v>25302.8122</v>
+      </c>
+      <c r="Z38" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y38:Y38),_xlfn.VSTACK($F$29,U38:U38))</f>
+        <v>7.500865757465365E-2</v>
+      </c>
+      <c r="AA38" s="13">
+        <f>(Y38+$J$29)/ABS($J$2)</f>
+        <v>4.1890751040333976E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>17</v>
       </c>
@@ -2706,19 +3066,44 @@
         <v>31.04</v>
       </c>
       <c r="J39" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>24406.441599999998</v>
       </c>
       <c r="K39" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>9.0772452950477617E-2</v>
       </c>
       <c r="L39" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2.7419400680945852E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R39" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T39" s="7"/>
+      <c r="U39" s="8">
+        <v>45901</v>
+      </c>
+      <c r="V39" s="5"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="9">
+        <v>339.79</v>
+      </c>
+      <c r="Y39" s="10">
+        <f>+X39*R39</f>
+        <v>86791.540330000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -2741,19 +3126,52 @@
         <v>31.74</v>
       </c>
       <c r="J40" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>24956.844599999997</v>
       </c>
       <c r="K40" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.10870504975318909</v>
       </c>
       <c r="L40" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3.6305317568289391E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R40" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T40" s="7"/>
+      <c r="U40" s="8">
+        <v>45931</v>
+      </c>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="9">
+        <v>33.630000000000003</v>
+      </c>
+      <c r="Y40" s="10">
+        <f>+X40*R40</f>
+        <v>26442.932700000001</v>
+      </c>
+      <c r="Z40" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y40:Y40),_xlfn.VSTACK($F$29,U40:U40))</f>
+        <v>0.1012986123561859</v>
+      </c>
+      <c r="AA40" s="13">
+        <f>(Y40+$J$29)/ABS($J$2)</f>
+        <v>6.0297293164117097E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
@@ -2776,19 +3194,44 @@
         <v>31.45</v>
       </c>
       <c r="J41" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>24728.820499999998</v>
       </c>
       <c r="K41" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>8.9758548140525821E-2</v>
       </c>
       <c r="L41" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3.2624009143532792E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R41" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T41" s="7"/>
+      <c r="U41" s="8">
+        <v>45931</v>
+      </c>
+      <c r="V41" s="5"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="9">
+        <v>343.46</v>
+      </c>
+      <c r="Y41" s="10">
+        <f>+X41*R41</f>
+        <v>87728.957419999992</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>17</v>
       </c>
@@ -2811,19 +3254,52 @@
         <v>29.71</v>
       </c>
       <c r="J42" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>23360.675899999998</v>
       </c>
       <c r="K42" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2.6664957404136665E-2</v>
       </c>
       <c r="L42" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.0536158594993078E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q42" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R42" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T42" s="7"/>
+      <c r="U42" s="8">
+        <v>45962</v>
+      </c>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="9">
+        <v>33.44</v>
+      </c>
+      <c r="Y42" s="10">
+        <f>+X42*R42</f>
+        <v>26293.537599999996</v>
+      </c>
+      <c r="Z42" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y42:Y42),_xlfn.VSTACK($F$29,U42:U42))</f>
+        <v>9.2157724499702456E-2</v>
+      </c>
+      <c r="AA42" s="13">
+        <f>(Y42+$J$29)/ABS($J$2)</f>
+        <v>5.7885401437552331E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>17</v>
       </c>
@@ -2846,19 +3322,44 @@
         <v>28.53</v>
       </c>
       <c r="J43" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>22432.8537</v>
       </c>
       <c r="K43" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>-1.0466119647026064E-2</v>
       </c>
       <c r="L43" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>-4.4429584436717707E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R43" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T43" s="7"/>
+      <c r="U43" s="8">
+        <v>45962</v>
+      </c>
+      <c r="V43" s="5"/>
+      <c r="W43" s="6"/>
+      <c r="X43" s="9">
+        <v>335.31</v>
+      </c>
+      <c r="Y43" s="10">
+        <f>+X43*R43</f>
+        <v>85647.227369999993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
@@ -2881,19 +3382,52 @@
         <v>30.01</v>
       </c>
       <c r="J44" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>23596.562900000001</v>
       </c>
       <c r="K44" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>3.1338271498680112E-2</v>
       </c>
       <c r="L44" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.4344408689568931E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R44" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T44" s="7"/>
+      <c r="U44" s="8">
+        <v>45992</v>
+      </c>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="9">
+        <v>33.11</v>
+      </c>
+      <c r="Y44" s="10">
+        <f>+X44*R44</f>
+        <v>26034.061899999997</v>
+      </c>
+      <c r="Z44" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y44:Y44),_xlfn.VSTACK($F$29,U44:U44))</f>
+        <v>8.1469628214836123E-2</v>
+      </c>
+      <c r="AA44" s="13">
+        <f>(Y44+$J$29)/ABS($J$2)</f>
+        <v>5.3696326333518951E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>17</v>
       </c>
@@ -2916,19 +3450,44 @@
         <v>29.99</v>
       </c>
       <c r="J45" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>23580.837099999997</v>
       </c>
       <c r="K45" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2.8850188851356512E-2</v>
       </c>
       <c r="L45" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.4090525349930482E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R45" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T45" s="7"/>
+      <c r="U45" s="8">
+        <v>45992</v>
+      </c>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="9">
+        <v>350.59</v>
+      </c>
+      <c r="Y45" s="10">
+        <f>+X45*R45</f>
+        <v>89550.151929999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>17</v>
       </c>
@@ -2951,19 +3510,52 @@
         <v>31.68</v>
       </c>
       <c r="J46" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>24909.6672</v>
       </c>
       <c r="K46" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>6.7782369256019603E-2</v>
       </c>
       <c r="L46" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3.5543667549374283E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P46" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R46" s="7">
+        <v>786.29</v>
+      </c>
+      <c r="S46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T46" s="7"/>
+      <c r="U46" s="8">
+        <v>46023</v>
+      </c>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="9">
+        <v>32.229999999999997</v>
+      </c>
+      <c r="Y46" s="10">
+        <f>+X46*R46</f>
+        <v>25342.126699999997</v>
+      </c>
+      <c r="Z46" s="13">
+        <f>XIRR(_xlfn.VSTACK($J$29,Y46:Y46),_xlfn.VSTACK($F$29,U46:U46))</f>
+        <v>6.18018299341202E-2</v>
+      </c>
+      <c r="AA46" s="13">
+        <f>(Y46+$J$29)/ABS($J$2)</f>
+        <v>4.2525459389429893E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>17</v>
       </c>
@@ -2986,19 +3578,44 @@
         <v>32.18</v>
       </c>
       <c r="J47" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>25302.8122</v>
       </c>
       <c r="K47" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>7.500865757465365E-2</v>
       </c>
       <c r="L47" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>4.1890751040333976E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R47" s="7">
+        <v>255.42699999999999</v>
+      </c>
+      <c r="S47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T47" s="7"/>
+      <c r="U47" s="8">
+        <v>46023</v>
+      </c>
+      <c r="V47" s="5"/>
+      <c r="W47" s="6"/>
+      <c r="X47" s="9">
+        <v>361.98</v>
+      </c>
+      <c r="Y47" s="10">
+        <f>+X47*R47</f>
+        <v>92459.465460000007</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>17</v>
       </c>
@@ -3021,15 +3638,15 @@
         <v>33.630000000000003</v>
       </c>
       <c r="J48" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>26442.932700000001</v>
       </c>
       <c r="K48" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.1012986123561859</v>
       </c>
       <c r="L48" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>6.0297293164117097E-2</v>
       </c>
     </row>
@@ -3056,15 +3673,15 @@
         <v>33.44</v>
       </c>
       <c r="J49" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>26293.537599999996</v>
       </c>
       <c r="K49" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>9.2157724499702456E-2</v>
       </c>
       <c r="L49" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>5.7885401437552331E-2</v>
       </c>
     </row>
@@ -3091,15 +3708,15 @@
         <v>33.11</v>
       </c>
       <c r="J50" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>26034.061899999997</v>
       </c>
       <c r="K50" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>8.1469628214836123E-2</v>
       </c>
       <c r="L50" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>5.3696326333518951E-2</v>
       </c>
     </row>
@@ -3126,15 +3743,15 @@
         <v>32.229999999999997</v>
       </c>
       <c r="J51" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>25342.126699999997</v>
       </c>
       <c r="K51" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>6.18018299341202E-2</v>
       </c>
       <c r="L51" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>4.2525459389429893E-2</v>
       </c>
     </row>
@@ -3145,11 +3762,16 @@
       <c r="F53" s="12"/>
     </row>
   </sheetData>
+  <autoFilter ref="P1:AA47" xr:uid="{840B4B52-5CB9-41B5-89C1-B1D0A0795C06}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P2:AA47">
+      <sortCondition ref="U1:U47"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I30:J53">
     <sortCondition descending="1" ref="J30:J53"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4:G24 G29 V2" xr:uid="{786B1B08-543B-41BE-8266-499A04655516}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4:G24 G29 V2:V3 V27:V47" xr:uid="{786B1B08-543B-41BE-8266-499A04655516}">
       <formula1>"Acquisto,Vendita,-"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>